<commit_message>
done with the problems
</commit_message>
<xml_diff>
--- a/2toy/large/results.xlsx
+++ b/2toy/large/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Scenarios</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Knitro s(gap)</t>
   </si>
   <si>
-    <t>Baron s(gap)</t>
-  </si>
-  <si>
     <t>Pajarito s(gap)</t>
   </si>
   <si>
@@ -62,13 +59,25 @@
     <t>Timed out(87%)</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Nodes</t>
   </si>
   <si>
     <t>Max Iterations</t>
+  </si>
+  <si>
+    <t>BARON s(gap)</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Master (s)</t>
+  </si>
+  <si>
+    <t>Subproblem (s)</t>
+  </si>
+  <si>
+    <t>UB subproblem (s)</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,13 +109,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -397,206 +437,252 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2">
+        <v>182</v>
+      </c>
+      <c r="C3" s="2">
+        <v>240</v>
+      </c>
+      <c r="D3" s="2">
+        <v>122</v>
+      </c>
+      <c r="E3" s="2">
+        <v>182</v>
+      </c>
+      <c r="F3" s="2">
+        <v>64</v>
+      </c>
+      <c r="G3" s="2">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>150</v>
+      </c>
+      <c r="B4" s="2">
+        <v>452</v>
+      </c>
+      <c r="C4" s="2">
+        <v>600</v>
+      </c>
+      <c r="D4" s="2">
+        <v>302</v>
+      </c>
+      <c r="E4" s="2">
+        <v>452</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>300</v>
+      </c>
+      <c r="B5" s="4">
+        <v>902</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="4">
+        <v>602</v>
+      </c>
+      <c r="E5" s="4">
+        <v>902</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4">
+        <v>987</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2">
+        <v>76</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F12" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>62</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>42</v>
-      </c>
-      <c r="E2">
-        <v>62</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1468</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>182</v>
-      </c>
-      <c r="C3">
-        <v>240</v>
-      </c>
-      <c r="D3">
-        <v>122</v>
-      </c>
-      <c r="E3">
-        <v>182</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>64</v>
-      </c>
-      <c r="H3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="G12" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>150</v>
       </c>
-      <c r="B4">
-        <v>452</v>
-      </c>
-      <c r="C4">
-        <v>600</v>
-      </c>
-      <c r="D4">
-        <v>302</v>
-      </c>
-      <c r="E4">
-        <v>452</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B13" s="2">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>81</v>
+      </c>
+      <c r="E13" s="2">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>300</v>
       </c>
-      <c r="B5">
-        <v>902</v>
-      </c>
-      <c r="C5">
-        <v>1200</v>
-      </c>
-      <c r="D5">
-        <v>602</v>
-      </c>
-      <c r="E5">
-        <v>902</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B14" s="4">
+        <v>121</v>
+      </c>
+      <c r="C14" s="4">
         <v>11</v>
       </c>
-      <c r="H5">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>80</v>
-      </c>
-      <c r="C11">
+      <c r="D14" s="4">
+        <v>81</v>
+      </c>
+      <c r="E14" s="4">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>60</v>
-      </c>
-      <c r="B12">
-        <v>76</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>150</v>
-      </c>
-      <c r="B13">
-        <v>111</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>300</v>
-      </c>
-      <c r="B14">
-        <v>121</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
+      <c r="G14" s="4">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add benchmark in gams for sbb and alphaecp
</commit_message>
<xml_diff>
--- a/2toy/large/results.xlsx
+++ b/2toy/large/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="38420" yWindow="2280" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Scenarios</t>
   </si>
@@ -78,19 +78,45 @@
   </si>
   <si>
     <t>UB subproblem (s)</t>
+  </si>
+  <si>
+    <t>SBB s(gap)</t>
+  </si>
+  <si>
+    <t>AlphaECP s(gap)</t>
+  </si>
+  <si>
+    <t>Timed out(7%)</t>
+  </si>
+  <si>
+    <t>Timed out(234%)</t>
+  </si>
+  <si>
+    <t>|bestbound-bestinteger|/(1e-10+|bestinteger|)</t>
+  </si>
+  <si>
+    <t>Timed out(245%)</t>
+  </si>
+  <si>
+    <t>Timed out(247%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF323232"/>
+      <name val="Courier New"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,6 +173,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,12 +467,13 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,16 +490,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>20</v>
       </c>
@@ -486,14 +524,20 @@
       <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
-        <v>5</v>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2">
+        <v>9</v>
       </c>
       <c r="J2" s="3">
         <v>1468</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>60</v>
       </c>
@@ -510,16 +554,22 @@
         <v>182</v>
       </c>
       <c r="F3" s="2">
-        <v>64</v>
-      </c>
-      <c r="G3" s="2">
         <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2">
+        <v>60</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>150</v>
       </c>
@@ -535,17 +585,23 @@
       <c r="E4" s="2">
         <v>452</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="F4" s="2">
         <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2">
+        <v>254</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>300</v>
       </c>
@@ -561,17 +617,23 @@
       <c r="E5" s="4">
         <v>902</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="F5" s="4">
         <v>987</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4">
+        <v>917</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>20</v>
       </c>
@@ -617,7 +679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>60</v>
       </c>
@@ -640,7 +702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>150</v>
       </c>
@@ -663,7 +725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>300</v>
       </c>
@@ -683,6 +745,11 @@
         <v>3</v>
       </c>
       <c r="G14" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J18" s="7" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish the first submission of the paper. all up to date
</commit_message>
<xml_diff>
--- a/2toy/large/results.xlsx
+++ b/2toy/large/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="2280" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="2280" windowWidth="33600" windowHeight="18940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Scenarios</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Timed out(247%)</t>
+  </si>
+  <si>
+    <t>DICOPT s(gap)</t>
+  </si>
+  <si>
+    <t>Timed out(9%)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,7 +179,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -455,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,13 +472,14 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,14 +495,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -504,8 +510,11 @@
       <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>20</v>
       </c>
@@ -521,14 +530,14 @@
       <c r="E2" s="2">
         <v>62</v>
       </c>
-      <c r="F2" s="2">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="G2" s="2">
+        <v>9</v>
+      </c>
       <c r="H2" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J2" s="3">
         <v>1468</v>
@@ -536,8 +545,11 @@
       <c r="K2" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>60</v>
       </c>
@@ -553,14 +565,14 @@
       <c r="E3" s="2">
         <v>182</v>
       </c>
-      <c r="F3" s="2">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="G3" s="2">
+        <v>60</v>
+      </c>
       <c r="H3" s="2">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>7</v>
@@ -568,8 +580,11 @@
       <c r="K3" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>150</v>
       </c>
@@ -585,14 +600,14 @@
       <c r="E4" s="2">
         <v>452</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>23</v>
+      <c r="G4" s="2">
+        <v>254</v>
       </c>
       <c r="H4" s="2">
-        <v>254</v>
+        <v>685</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
@@ -600,8 +615,11 @@
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>300</v>
       </c>
@@ -617,14 +635,14 @@
       <c r="E5" s="4">
         <v>902</v>
       </c>
-      <c r="F5" s="4">
-        <v>987</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="4">
+      <c r="G5" s="4">
         <v>917</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>8</v>
@@ -632,8 +650,11 @@
       <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="4">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>20</v>
       </c>
@@ -679,7 +700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>60</v>
       </c>
@@ -702,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>150</v>
       </c>
@@ -725,7 +746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>300</v>
       </c>
@@ -749,7 +770,7 @@
       </c>
     </row>
     <row r="18" spans="10:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>